<commit_message>
adding comments to RAData, images of interface
</commit_message>
<xml_diff>
--- a/RoboRA/RAData fields.xlsx
+++ b/RoboRA/RAData fields.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JSNOEYIN\excelSQL\RoboRA\"/>
@@ -196,7 +196,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="308">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="508" uniqueCount="314">
   <si>
     <t>dd_rcom_date</t>
   </si>
@@ -1242,6 +1242,24 @@
   </si>
   <si>
     <t># ad hoc (mail) reviews - blank if zero.</t>
+  </si>
+  <si>
+    <t>hasE</t>
+  </si>
+  <si>
+    <t>TRUE if has an E (or E/V) review. PAM is ambiguous if RAs must explain E/V reviews.</t>
+  </si>
+  <si>
+    <t>reviewers in FL review system</t>
+  </si>
+  <si>
+    <t>Change name of signer of RA.  When RoboRA pref=PD, this is the PD name from eJ.</t>
+  </si>
+  <si>
+    <t>Second line of RA signature. Change on RoboRA Prefs or individually on RAData.</t>
+  </si>
+  <si>
+    <t>Panel recommendation spelled out</t>
   </si>
 </sst>
 </file>
@@ -1509,8 +1527,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E138" totalsRowShown="0">
-  <autoFilter ref="A3:E138"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A3:E139" totalsRowShown="0">
   <tableColumns count="5">
     <tableColumn id="1" name="col#"/>
     <tableColumn id="2" name="field" dataDxfId="2"/>
@@ -1819,10 +1836,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:E138"/>
+  <sheetPr codeName="Sheet1"/>
+  <dimension ref="A3:E139"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E48" sqref="E48"/>
+      <selection activeCell="D45" sqref="D45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -1962,7 +1980,9 @@
       <c r="D10" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="E10" s="21"/>
+      <c r="E10" s="21" t="s">
+        <v>313</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A11">
@@ -2174,7 +2194,9 @@
       <c r="D24" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E24" s="21"/>
+      <c r="E24" s="21" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A25">
@@ -2186,7 +2208,9 @@
       <c r="D25" s="2" t="s">
         <v>170</v>
       </c>
-      <c r="E25" s="21"/>
+      <c r="E25" s="21" t="s">
+        <v>312</v>
+      </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A26">
@@ -2362,6 +2386,9 @@
       <c r="C36" t="s">
         <v>275</v>
       </c>
+      <c r="D36" s="4" t="s">
+        <v>310</v>
+      </c>
       <c r="E36" s="21" t="s">
         <v>250</v>
       </c>
@@ -2376,6 +2403,9 @@
       <c r="C37" t="s">
         <v>275</v>
       </c>
+      <c r="D37" s="4" t="s">
+        <v>310</v>
+      </c>
       <c r="E37" s="21" t="s">
         <v>251</v>
       </c>
@@ -2390,6 +2420,9 @@
       <c r="C38" t="s">
         <v>275</v>
       </c>
+      <c r="D38" s="4" t="s">
+        <v>310</v>
+      </c>
       <c r="E38" s="21" t="s">
         <v>249</v>
       </c>
@@ -2404,6 +2437,9 @@
       <c r="C39" t="s">
         <v>276</v>
       </c>
+      <c r="D39" s="4" t="s">
+        <v>310</v>
+      </c>
       <c r="E39" s="21" t="s">
         <v>262</v>
       </c>
@@ -2412,84 +2448,85 @@
       <c r="A40">
         <v>37</v>
       </c>
-      <c r="B40" s="17" t="s">
-        <v>36</v>
+      <c r="B40" s="14" t="s">
+        <v>308</v>
       </c>
       <c r="C40" t="s">
-        <v>275</v>
-      </c>
+        <v>164</v>
+      </c>
+      <c r="D40" s="5"/>
       <c r="E40" s="21" t="s">
-        <v>263</v>
+        <v>309</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A41">
         <v>38</v>
       </c>
-      <c r="B41" s="18" t="s">
-        <v>37</v>
+      <c r="B41" s="17" t="s">
+        <v>36</v>
       </c>
       <c r="C41" t="s">
-        <v>139</v>
+        <v>275</v>
       </c>
       <c r="E41" s="21" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A42">
         <v>39</v>
       </c>
-      <c r="B42" s="19" t="s">
-        <v>38</v>
+      <c r="B42" s="18" t="s">
+        <v>37</v>
       </c>
       <c r="C42" t="s">
-        <v>278</v>
+        <v>139</v>
       </c>
       <c r="E42" s="21" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A43">
         <v>40</v>
       </c>
-      <c r="B43" s="9" t="s">
-        <v>39</v>
+      <c r="B43" s="19" t="s">
+        <v>38</v>
       </c>
       <c r="C43" t="s">
         <v>278</v>
       </c>
       <c r="E43" s="21" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A44">
         <v>41</v>
       </c>
-      <c r="B44" s="17" t="s">
-        <v>40</v>
+      <c r="B44" s="9" t="s">
+        <v>39</v>
       </c>
       <c r="C44" t="s">
-        <v>139</v>
+        <v>278</v>
       </c>
       <c r="E44" s="21" t="s">
-        <v>303</v>
+        <v>248</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A45">
         <v>42</v>
       </c>
-      <c r="B45" s="15" t="s">
-        <v>41</v>
+      <c r="B45" s="17" t="s">
+        <v>40</v>
       </c>
       <c r="C45" t="s">
         <v>139</v>
       </c>
       <c r="E45" s="21" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.4">
@@ -2497,16 +2534,13 @@
         <v>43</v>
       </c>
       <c r="B46" s="15" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C46" t="s">
         <v>139</v>
       </c>
-      <c r="D46" s="3" t="s">
-        <v>283</v>
-      </c>
       <c r="E46" s="21" t="s">
-        <v>284</v>
+        <v>304</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.4">
@@ -2514,13 +2548,16 @@
         <v>44</v>
       </c>
       <c r="B47" s="15" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C47" t="s">
-        <v>275</v>
+        <v>139</v>
+      </c>
+      <c r="D47" s="3" t="s">
+        <v>283</v>
       </c>
       <c r="E47" s="21" t="s">
-        <v>307</v>
+        <v>284</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.4">
@@ -2528,44 +2565,41 @@
         <v>45</v>
       </c>
       <c r="B48" s="15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C48" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="E48" s="21" t="s">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A49">
         <v>46</v>
       </c>
-      <c r="B49" s="7" t="s">
-        <v>45</v>
+      <c r="B49" s="15" t="s">
+        <v>44</v>
       </c>
       <c r="C49" t="s">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="E49" s="21" t="s">
-        <v>305</v>
+        <v>306</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A50">
         <v>47</v>
       </c>
-      <c r="B50" s="15" t="s">
-        <v>46</v>
+      <c r="B50" s="7" t="s">
+        <v>45</v>
       </c>
       <c r="C50" t="s">
-        <v>299</v>
-      </c>
-      <c r="D50" s="5" t="s">
-        <v>152</v>
+        <v>275</v>
       </c>
       <c r="E50" s="21" t="s">
-        <v>281</v>
+        <v>305</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.4">
@@ -2573,16 +2607,16 @@
         <v>48</v>
       </c>
       <c r="B51" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C51" t="s">
-        <v>253</v>
-      </c>
-      <c r="D51" s="4" t="s">
-        <v>162</v>
+        <v>299</v>
+      </c>
+      <c r="D51" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E51" s="21" t="s">
-        <v>252</v>
+        <v>281</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.4">
@@ -2590,16 +2624,16 @@
         <v>49</v>
       </c>
       <c r="B52" s="15" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C52" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E52" s="21" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.4">
@@ -2607,50 +2641,50 @@
         <v>50</v>
       </c>
       <c r="B53" s="15" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="C53" t="s">
-        <v>297</v>
-      </c>
-      <c r="D53" s="5" t="s">
-        <v>152</v>
+        <v>260</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E53" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A54">
         <v>51</v>
       </c>
-      <c r="B54" s="7" t="s">
-        <v>50</v>
+      <c r="B54" s="15" t="s">
+        <v>49</v>
       </c>
       <c r="C54" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D54" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E54" s="21" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A55">
         <v>52</v>
       </c>
-      <c r="B55" s="15" t="s">
-        <v>51</v>
+      <c r="B55" s="7" t="s">
+        <v>50</v>
       </c>
       <c r="C55" t="s">
-        <v>276</v>
-      </c>
-      <c r="D55" s="4" t="s">
-        <v>162</v>
+        <v>298</v>
+      </c>
+      <c r="D55" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E55" s="21" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.4">
@@ -2658,50 +2692,50 @@
         <v>53</v>
       </c>
       <c r="B56" s="15" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C56" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E56" s="21" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A57">
         <v>54</v>
       </c>
-      <c r="B57" s="20" t="s">
-        <v>53</v>
+      <c r="B57" s="15" t="s">
+        <v>52</v>
       </c>
       <c r="C57" t="s">
-        <v>279</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>152</v>
+        <v>277</v>
+      </c>
+      <c r="D57" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E57" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A58">
         <v>55</v>
       </c>
-      <c r="B58" s="15" t="s">
-        <v>54</v>
+      <c r="B58" s="20" t="s">
+        <v>53</v>
       </c>
       <c r="C58" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D58" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E58" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.4">
@@ -2709,16 +2743,16 @@
         <v>56</v>
       </c>
       <c r="B59" s="15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C59" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="D59" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E59" s="21" t="s">
-        <v>280</v>
+        <v>267</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.4">
@@ -2726,16 +2760,16 @@
         <v>57</v>
       </c>
       <c r="B60" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C60" t="s">
-        <v>253</v>
-      </c>
-      <c r="D60" s="4" t="s">
-        <v>162</v>
+        <v>299</v>
+      </c>
+      <c r="D60" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E60" s="21" t="s">
-        <v>252</v>
+        <v>280</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.4">
@@ -2743,16 +2777,16 @@
         <v>58</v>
       </c>
       <c r="B61" s="15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C61" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D61" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E61" s="21" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.4">
@@ -2760,50 +2794,50 @@
         <v>59</v>
       </c>
       <c r="B62" s="15" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C62" t="s">
-        <v>297</v>
-      </c>
-      <c r="D62" s="5" t="s">
-        <v>152</v>
+        <v>260</v>
+      </c>
+      <c r="D62" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E62" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A63">
         <v>60</v>
       </c>
-      <c r="B63" s="7" t="s">
-        <v>59</v>
+      <c r="B63" s="15" t="s">
+        <v>58</v>
       </c>
       <c r="C63" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D63" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E63" s="21" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A64">
         <v>61</v>
       </c>
-      <c r="B64" s="15" t="s">
-        <v>60</v>
+      <c r="B64" s="7" t="s">
+        <v>59</v>
       </c>
       <c r="C64" t="s">
-        <v>276</v>
-      </c>
-      <c r="D64" s="4" t="s">
-        <v>162</v>
+        <v>298</v>
+      </c>
+      <c r="D64" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E64" s="21" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.4">
@@ -2811,16 +2845,16 @@
         <v>62</v>
       </c>
       <c r="B65" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C65" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D65" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E65" s="21" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.4">
@@ -2828,16 +2862,16 @@
         <v>63</v>
       </c>
       <c r="B66" s="15" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C66" t="s">
-        <v>279</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>152</v>
+        <v>277</v>
+      </c>
+      <c r="D66" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E66" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.4">
@@ -2845,16 +2879,16 @@
         <v>64</v>
       </c>
       <c r="B67" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C67" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D67" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E67" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.4">
@@ -2862,16 +2896,16 @@
         <v>65</v>
       </c>
       <c r="B68" s="15" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C68" t="s">
-        <v>299</v>
+        <v>275</v>
       </c>
       <c r="D68" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E68" s="21" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.4">
@@ -2879,16 +2913,16 @@
         <v>66</v>
       </c>
       <c r="B69" s="15" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C69" t="s">
-        <v>253</v>
-      </c>
-      <c r="D69" s="4" t="s">
-        <v>162</v>
+        <v>299</v>
+      </c>
+      <c r="D69" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E69" s="21" t="s">
-        <v>252</v>
+        <v>282</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.4">
@@ -2896,16 +2930,16 @@
         <v>67</v>
       </c>
       <c r="B70" s="15" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C70" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="D70" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E70" s="21" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.4">
@@ -2913,50 +2947,50 @@
         <v>68</v>
       </c>
       <c r="B71" s="15" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C71" t="s">
-        <v>297</v>
-      </c>
-      <c r="D71" s="5" t="s">
-        <v>152</v>
+        <v>260</v>
+      </c>
+      <c r="D71" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E71" s="21" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A72">
         <v>69</v>
       </c>
-      <c r="B72" s="7" t="s">
-        <v>68</v>
+      <c r="B72" s="15" t="s">
+        <v>67</v>
       </c>
       <c r="C72" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="D72" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E72" s="21" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A73">
         <v>70</v>
       </c>
-      <c r="B73" s="15" t="s">
-        <v>69</v>
+      <c r="B73" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="C73" t="s">
-        <v>276</v>
-      </c>
-      <c r="D73" s="4" t="s">
-        <v>162</v>
+        <v>298</v>
+      </c>
+      <c r="D73" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E73" s="21" t="s">
-        <v>261</v>
+        <v>264</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.4">
@@ -2964,16 +2998,16 @@
         <v>71</v>
       </c>
       <c r="B74" s="15" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C74" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D74" s="4" t="s">
         <v>162</v>
       </c>
       <c r="E74" s="21" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.4">
@@ -2981,16 +3015,16 @@
         <v>72</v>
       </c>
       <c r="B75" s="15" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C75" t="s">
-        <v>279</v>
-      </c>
-      <c r="D75" s="5" t="s">
-        <v>152</v>
+        <v>277</v>
+      </c>
+      <c r="D75" s="4" t="s">
+        <v>162</v>
       </c>
       <c r="E75" s="21" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.4">
@@ -2998,47 +3032,47 @@
         <v>73</v>
       </c>
       <c r="B76" s="15" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C76" t="s">
-        <v>275</v>
+        <v>279</v>
       </c>
       <c r="D76" s="5" t="s">
         <v>152</v>
       </c>
       <c r="E76" s="21" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A77">
         <v>74</v>
       </c>
-      <c r="B77" s="9" t="s">
-        <v>73</v>
+      <c r="B77" s="15" t="s">
+        <v>72</v>
       </c>
       <c r="C77" t="s">
-        <v>296</v>
+        <v>275</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>152</v>
       </c>
       <c r="E77" s="21" t="s">
-        <v>179</v>
+        <v>267</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A78">
         <v>75</v>
       </c>
-      <c r="B78" s="15" t="s">
-        <v>74</v>
+      <c r="B78" s="9" t="s">
+        <v>73</v>
       </c>
       <c r="C78" t="s">
-        <v>294</v>
-      </c>
-      <c r="D78" s="3" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="E78" s="21" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.4">
@@ -3046,16 +3080,16 @@
         <v>76</v>
       </c>
       <c r="B79" s="15" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C79" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D79" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E79" s="21" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.4">
@@ -3063,30 +3097,33 @@
         <v>77</v>
       </c>
       <c r="B80" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C80" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D80" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E80" s="21" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A81">
         <v>78</v>
       </c>
-      <c r="B81" s="19" t="s">
-        <v>77</v>
+      <c r="B81" s="15" t="s">
+        <v>76</v>
       </c>
       <c r="C81" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D81" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E81" s="21" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.4">
@@ -3094,47 +3131,47 @@
         <v>79</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="C82" t="s">
-        <v>301</v>
-      </c>
-      <c r="D82" s="4" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="E82" s="21" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A83">
         <v>80</v>
       </c>
-      <c r="B83" s="9" t="s">
-        <v>79</v>
+      <c r="B83" s="19" t="s">
+        <v>78</v>
       </c>
       <c r="C83" t="s">
-        <v>302</v>
-      </c>
-      <c r="D83" s="3" t="s">
-        <v>185</v>
+        <v>301</v>
+      </c>
+      <c r="D83" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="E83" s="21" t="s">
-        <v>225</v>
+        <v>184</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A84">
         <v>81</v>
       </c>
-      <c r="B84" s="15" t="s">
-        <v>80</v>
+      <c r="B84" s="9" t="s">
+        <v>79</v>
       </c>
       <c r="C84" t="s">
-        <v>296</v>
+        <v>302</v>
+      </c>
+      <c r="D84" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E84" s="21" t="s">
-        <v>189</v>
+        <v>225</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.4">
@@ -3142,33 +3179,30 @@
         <v>82</v>
       </c>
       <c r="B85" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C85" t="s">
-        <v>294</v>
-      </c>
-      <c r="D85" s="3" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="E85" s="21" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="86" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A86">
         <v>83</v>
       </c>
-      <c r="B86" s="20" t="s">
-        <v>82</v>
+      <c r="B86" s="15" t="s">
+        <v>81</v>
       </c>
       <c r="C86" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D86" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E86" s="21" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="87" spans="1:5" x14ac:dyDescent="0.4">
@@ -3176,30 +3210,33 @@
         <v>84</v>
       </c>
       <c r="B87" s="20" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="C87" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D87" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E87" s="21" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="88" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A88">
         <v>85</v>
       </c>
-      <c r="B88" s="19" t="s">
-        <v>84</v>
+      <c r="B88" s="20" t="s">
+        <v>83</v>
       </c>
       <c r="C88" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D88" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E88" s="21" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="89" spans="1:5" x14ac:dyDescent="0.4">
@@ -3207,47 +3244,47 @@
         <v>86</v>
       </c>
       <c r="B89" s="19" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C89" t="s">
-        <v>301</v>
-      </c>
-      <c r="D89" s="4" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="E89" s="21" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="90" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A90">
         <v>87</v>
       </c>
-      <c r="B90" s="9" t="s">
-        <v>86</v>
+      <c r="B90" s="19" t="s">
+        <v>85</v>
       </c>
       <c r="C90" t="s">
-        <v>302</v>
-      </c>
-      <c r="D90" s="3" t="s">
-        <v>185</v>
+        <v>301</v>
+      </c>
+      <c r="D90" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="E90" s="21" t="s">
-        <v>226</v>
+        <v>194</v>
       </c>
     </row>
     <row r="91" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A91">
         <v>88</v>
       </c>
-      <c r="B91" s="15" t="s">
-        <v>87</v>
+      <c r="B91" s="9" t="s">
+        <v>86</v>
       </c>
       <c r="C91" t="s">
-        <v>296</v>
+        <v>302</v>
+      </c>
+      <c r="D91" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E91" s="21" t="s">
-        <v>195</v>
+        <v>226</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.4">
@@ -3255,33 +3292,30 @@
         <v>89</v>
       </c>
       <c r="B92" s="15" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C92" t="s">
-        <v>294</v>
-      </c>
-      <c r="D92" s="3" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="E92" s="21" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A93">
         <v>90</v>
       </c>
-      <c r="B93" s="20" t="s">
-        <v>89</v>
+      <c r="B93" s="15" t="s">
+        <v>88</v>
       </c>
       <c r="C93" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D93" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E93" s="21" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.4">
@@ -3289,30 +3323,33 @@
         <v>91</v>
       </c>
       <c r="B94" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C94" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D94" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E94" s="21" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="95" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A95">
         <v>92</v>
       </c>
-      <c r="B95" s="19" t="s">
-        <v>91</v>
+      <c r="B95" s="20" t="s">
+        <v>90</v>
       </c>
       <c r="C95" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D95" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E95" s="21" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.4">
@@ -3320,47 +3357,47 @@
         <v>93</v>
       </c>
       <c r="B96" s="19" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C96" t="s">
-        <v>301</v>
-      </c>
-      <c r="D96" s="4" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="E96" s="21" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A97">
         <v>94</v>
       </c>
-      <c r="B97" s="9" t="s">
-        <v>93</v>
+      <c r="B97" s="19" t="s">
+        <v>92</v>
       </c>
       <c r="C97" t="s">
-        <v>302</v>
-      </c>
-      <c r="D97" s="3" t="s">
-        <v>185</v>
+        <v>301</v>
+      </c>
+      <c r="D97" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="E97" s="21" t="s">
-        <v>227</v>
+        <v>200</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A98">
         <v>95</v>
       </c>
-      <c r="B98" s="15" t="s">
-        <v>94</v>
+      <c r="B98" s="9" t="s">
+        <v>93</v>
       </c>
       <c r="C98" t="s">
-        <v>296</v>
+        <v>302</v>
+      </c>
+      <c r="D98" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E98" s="21" t="s">
-        <v>201</v>
+        <v>227</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.4">
@@ -3368,33 +3405,30 @@
         <v>96</v>
       </c>
       <c r="B99" s="15" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C99" t="s">
-        <v>294</v>
-      </c>
-      <c r="D99" s="3" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="E99" s="21" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A100">
         <v>97</v>
       </c>
-      <c r="B100" s="20" t="s">
-        <v>96</v>
+      <c r="B100" s="15" t="s">
+        <v>95</v>
       </c>
       <c r="C100" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D100" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E100" s="21" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.4">
@@ -3402,30 +3436,33 @@
         <v>98</v>
       </c>
       <c r="B101" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C101" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D101" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E101" s="21" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A102">
         <v>99</v>
       </c>
-      <c r="B102" s="19" t="s">
-        <v>98</v>
+      <c r="B102" s="20" t="s">
+        <v>97</v>
       </c>
       <c r="C102" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D102" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E102" s="21" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.4">
@@ -3433,47 +3470,47 @@
         <v>100</v>
       </c>
       <c r="B103" s="19" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C103" t="s">
-        <v>301</v>
-      </c>
-      <c r="D103" s="4" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="E103" s="21" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A104">
         <v>101</v>
       </c>
-      <c r="B104" s="9" t="s">
-        <v>100</v>
+      <c r="B104" s="19" t="s">
+        <v>99</v>
       </c>
       <c r="C104" t="s">
-        <v>302</v>
-      </c>
-      <c r="D104" s="3" t="s">
-        <v>185</v>
+        <v>301</v>
+      </c>
+      <c r="D104" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="E104" s="21" t="s">
-        <v>228</v>
+        <v>206</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A105">
         <v>102</v>
       </c>
-      <c r="B105" s="15" t="s">
-        <v>101</v>
+      <c r="B105" s="9" t="s">
+        <v>100</v>
       </c>
       <c r="C105" t="s">
-        <v>296</v>
+        <v>302</v>
+      </c>
+      <c r="D105" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E105" s="21" t="s">
-        <v>207</v>
+        <v>228</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.4">
@@ -3481,33 +3518,30 @@
         <v>103</v>
       </c>
       <c r="B106" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C106" t="s">
-        <v>294</v>
-      </c>
-      <c r="D106" s="3" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="E106" s="21" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A107">
         <v>104</v>
       </c>
-      <c r="B107" s="20" t="s">
-        <v>103</v>
+      <c r="B107" s="15" t="s">
+        <v>102</v>
       </c>
       <c r="C107" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D107" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E107" s="21" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.4">
@@ -3515,30 +3549,33 @@
         <v>105</v>
       </c>
       <c r="B108" s="20" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C108" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D108" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E108" s="21" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A109">
         <v>106</v>
       </c>
-      <c r="B109" s="19" t="s">
-        <v>105</v>
+      <c r="B109" s="20" t="s">
+        <v>104</v>
       </c>
       <c r="C109" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D109" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E109" s="21" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.4">
@@ -3546,47 +3583,47 @@
         <v>107</v>
       </c>
       <c r="B110" s="19" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C110" t="s">
-        <v>301</v>
-      </c>
-      <c r="D110" s="4" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="E110" s="21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A111">
         <v>108</v>
       </c>
-      <c r="B111" s="9" t="s">
-        <v>107</v>
+      <c r="B111" s="19" t="s">
+        <v>106</v>
       </c>
       <c r="C111" t="s">
-        <v>302</v>
-      </c>
-      <c r="D111" s="3" t="s">
-        <v>185</v>
+        <v>301</v>
+      </c>
+      <c r="D111" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="E111" s="21" t="s">
-        <v>229</v>
+        <v>212</v>
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A112">
         <v>109</v>
       </c>
-      <c r="B112" s="15" t="s">
-        <v>108</v>
+      <c r="B112" s="9" t="s">
+        <v>107</v>
       </c>
       <c r="C112" t="s">
-        <v>296</v>
+        <v>302</v>
+      </c>
+      <c r="D112" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E112" s="21" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.4">
@@ -3594,33 +3631,30 @@
         <v>110</v>
       </c>
       <c r="B113" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C113" t="s">
-        <v>294</v>
-      </c>
-      <c r="D113" s="3" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="E113" s="21" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A114">
         <v>111</v>
       </c>
-      <c r="B114" s="20" t="s">
-        <v>110</v>
+      <c r="B114" s="15" t="s">
+        <v>109</v>
       </c>
       <c r="C114" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D114" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E114" s="21" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.4">
@@ -3628,30 +3662,33 @@
         <v>112</v>
       </c>
       <c r="B115" s="20" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C115" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D115" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E115" s="21" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A116">
         <v>113</v>
       </c>
-      <c r="B116" s="19" t="s">
-        <v>112</v>
+      <c r="B116" s="20" t="s">
+        <v>111</v>
       </c>
       <c r="C116" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D116" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E116" s="21" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.4">
@@ -3659,47 +3696,47 @@
         <v>114</v>
       </c>
       <c r="B117" s="19" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="C117" t="s">
-        <v>301</v>
-      </c>
-      <c r="D117" s="4" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="E117" s="21" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A118">
         <v>115</v>
       </c>
-      <c r="B118" s="9" t="s">
-        <v>114</v>
+      <c r="B118" s="19" t="s">
+        <v>113</v>
       </c>
       <c r="C118" t="s">
-        <v>302</v>
-      </c>
-      <c r="D118" s="3" t="s">
-        <v>185</v>
+        <v>301</v>
+      </c>
+      <c r="D118" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="E118" s="21" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A119">
         <v>116</v>
       </c>
-      <c r="B119" s="15" t="s">
-        <v>115</v>
+      <c r="B119" s="9" t="s">
+        <v>114</v>
       </c>
       <c r="C119" t="s">
-        <v>296</v>
+        <v>302</v>
+      </c>
+      <c r="D119" s="3" t="s">
+        <v>185</v>
       </c>
       <c r="E119" s="21" t="s">
-        <v>219</v>
+        <v>230</v>
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.4">
@@ -3707,33 +3744,30 @@
         <v>117</v>
       </c>
       <c r="B120" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="C120" t="s">
-        <v>294</v>
-      </c>
-      <c r="D120" s="3" t="s">
-        <v>186</v>
+        <v>296</v>
       </c>
       <c r="E120" s="21" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A121">
         <v>118</v>
       </c>
-      <c r="B121" s="20" t="s">
-        <v>117</v>
+      <c r="B121" s="15" t="s">
+        <v>116</v>
       </c>
       <c r="C121" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
       <c r="D121" s="3" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="E121" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.4">
@@ -3741,30 +3775,33 @@
         <v>119</v>
       </c>
       <c r="B122" s="20" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C122" t="s">
-        <v>293</v>
+        <v>295</v>
       </c>
       <c r="D122" s="3" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="E122" s="21" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A123">
         <v>120</v>
       </c>
-      <c r="B123" s="19" t="s">
-        <v>119</v>
+      <c r="B123" s="20" t="s">
+        <v>118</v>
       </c>
       <c r="C123" t="s">
-        <v>300</v>
+        <v>293</v>
+      </c>
+      <c r="D123" s="3" t="s">
+        <v>186</v>
       </c>
       <c r="E123" s="21" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.4">
@@ -3772,33 +3809,30 @@
         <v>121</v>
       </c>
       <c r="B124" s="19" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C124" t="s">
-        <v>301</v>
-      </c>
-      <c r="D124" s="4" t="s">
-        <v>188</v>
+        <v>300</v>
       </c>
       <c r="E124" s="21" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A125">
         <v>122</v>
       </c>
-      <c r="B125" s="9" t="s">
-        <v>121</v>
+      <c r="B125" s="19" t="s">
+        <v>120</v>
       </c>
       <c r="C125" t="s">
-        <v>302</v>
-      </c>
-      <c r="D125" s="3" t="s">
-        <v>185</v>
+        <v>301</v>
+      </c>
+      <c r="D125" s="4" t="s">
+        <v>188</v>
       </c>
       <c r="E125" s="21" t="s">
-        <v>231</v>
+        <v>224</v>
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.4">
@@ -3806,16 +3840,16 @@
         <v>123</v>
       </c>
       <c r="B126" s="9" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C126" t="s">
-        <v>236</v>
+        <v>302</v>
       </c>
       <c r="D126" s="3" t="s">
-        <v>171</v>
+        <v>185</v>
       </c>
       <c r="E126" s="21" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.4">
@@ -3823,16 +3857,16 @@
         <v>124</v>
       </c>
       <c r="B127" s="9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C127" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="D127" s="3" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="E127" s="21" t="s">
-        <v>234</v>
+        <v>235</v>
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.4">
@@ -3840,16 +3874,16 @@
         <v>125</v>
       </c>
       <c r="B128" s="9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C128" t="s">
-        <v>178</v>
+        <v>238</v>
       </c>
       <c r="D128" s="3" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="E128" s="21" t="s">
-        <v>237</v>
+        <v>234</v>
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.4">
@@ -3857,13 +3891,16 @@
         <v>126</v>
       </c>
       <c r="B129" s="9" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C129" t="s">
-        <v>165</v>
+        <v>178</v>
+      </c>
+      <c r="D129" s="3" t="s">
+        <v>173</v>
       </c>
       <c r="E129" s="21" t="s">
-        <v>288</v>
+        <v>237</v>
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.4">
@@ -3871,16 +3908,13 @@
         <v>127</v>
       </c>
       <c r="B130" s="9" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C130" t="s">
-        <v>147</v>
-      </c>
-      <c r="D130" s="3" t="s">
-        <v>175</v>
+        <v>165</v>
       </c>
       <c r="E130" s="21" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.4">
@@ -3888,13 +3922,16 @@
         <v>128</v>
       </c>
       <c r="B131" s="9" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C131" t="s">
-        <v>146</v>
+        <v>147</v>
+      </c>
+      <c r="D131" s="3" t="s">
+        <v>175</v>
       </c>
       <c r="E131" s="21" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.4">
@@ -3902,16 +3939,13 @@
         <v>129</v>
       </c>
       <c r="B132" s="9" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C132" t="s">
-        <v>153</v>
-      </c>
-      <c r="D132" s="3" t="s">
-        <v>174</v>
+        <v>146</v>
       </c>
       <c r="E132" s="21" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.4">
@@ -3919,16 +3953,16 @@
         <v>130</v>
       </c>
       <c r="B133" s="9" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C133" t="s">
-        <v>239</v>
+        <v>153</v>
       </c>
       <c r="D133" s="3" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="E133" s="21" t="s">
-        <v>233</v>
+        <v>291</v>
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.4">
@@ -3936,44 +3970,44 @@
         <v>131</v>
       </c>
       <c r="B134" s="9" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C134" t="s">
-        <v>238</v>
+        <v>239</v>
       </c>
       <c r="D134" s="3" t="s">
         <v>172</v>
       </c>
       <c r="E134" s="21" t="s">
-        <v>232</v>
+        <v>233</v>
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A135">
         <v>132</v>
       </c>
-      <c r="B135" s="8" t="s">
-        <v>131</v>
+      <c r="B135" s="9" t="s">
+        <v>130</v>
+      </c>
+      <c r="C135" t="s">
+        <v>238</v>
+      </c>
+      <c r="D135" s="3" t="s">
+        <v>172</v>
       </c>
       <c r="E135" s="21" t="s">
-        <v>292</v>
+        <v>232</v>
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.4">
       <c r="A136">
         <v>133</v>
       </c>
-      <c r="B136" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="C136" t="s">
-        <v>177</v>
-      </c>
-      <c r="D136" s="5" t="s">
-        <v>152</v>
+      <c r="B136" s="8" t="s">
+        <v>131</v>
       </c>
       <c r="E136" s="21" t="s">
-        <v>156</v>
+        <v>292</v>
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.4">
@@ -3981,7 +4015,7 @@
         <v>134</v>
       </c>
       <c r="B137" s="9" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C137" t="s">
         <v>177</v>
@@ -3990,7 +4024,7 @@
         <v>152</v>
       </c>
       <c r="E137" s="21" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.4">
@@ -3998,7 +4032,7 @@
         <v>135</v>
       </c>
       <c r="B138" s="9" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="C138" t="s">
         <v>177</v>
@@ -4007,6 +4041,23 @@
         <v>152</v>
       </c>
       <c r="E138" s="21" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="139" spans="1:5" x14ac:dyDescent="0.4">
+      <c r="A139">
+        <v>136</v>
+      </c>
+      <c r="B139" s="9" t="s">
+        <v>134</v>
+      </c>
+      <c r="C139" t="s">
+        <v>177</v>
+      </c>
+      <c r="D139" s="5" t="s">
+        <v>152</v>
+      </c>
+      <c r="E139" s="21" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>